<commit_message>
removing verify by super admin
</commit_message>
<xml_diff>
--- a/superadmin/PHPExcel/test.xlsx
+++ b/superadmin/PHPExcel/test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\cutmCCCDC\superadmin\PHPExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\mygatecutm\superadmin\PHPExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA6E5F59-14E9-45DA-A9A3-036EDAC7BC3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AADF613-4EAE-4F2F-97BE-5DF2FAA569E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{743BF52B-2C3A-4DC4-A3A6-ECE32DFE79A7}"/>
   </bookViews>
@@ -25,39 +25,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>regd</t>
-  </si>
-  <si>
     <t>chinmaya</t>
   </si>
   <si>
-    <t>210720100009@cutm.ac.in</t>
-  </si>
-  <si>
-    <t>Applied Science</t>
-  </si>
-  <si>
-    <t>mca</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Campus</t>
-  </si>
-  <si>
-    <t>School</t>
-  </si>
-  <si>
-    <t>Dept</t>
-  </si>
-  <si>
     <t>BBSR</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>campus</t>
+  </si>
+  <si>
+    <t>situ@chinmayakumarbiswal.in</t>
   </si>
 </sst>
 </file>
@@ -440,12 +425,14 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.88671875" customWidth="1"/>
     <col min="10" max="10" width="12.6640625" customWidth="1"/>
     <col min="13" max="13" width="10.33203125" bestFit="1" customWidth="1"/>
@@ -457,20 +444,14 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>9</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -482,22 +463,13 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>210720100009</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
       </c>
       <c r="M2" s="3"/>
     </row>
@@ -506,7 +478,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{7EC17915-A6E6-428A-ACBC-71D7B6603314}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{0CB85A99-9EBD-43FF-9A68-800226806397}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>